<commit_message>
Updation of Emp Profile
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="12">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-12-06T09:13:59.345</t>
+  </si>
+  <si>
+    <t>ROLE GROUP : RTGO Operator 2023-12-06T06:31:26.060</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Automation Test Report - Build v4.22.00.158
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="18">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -81,6 +81,25 @@
   </si>
   <si>
     <t>ROLE GROUP : null</t>
+  </si>
+  <si>
+    <t>92457737 - Lilliana Williamson
+ROLE : RTGO100 1701844270281</t>
+  </si>
+  <si>
+    <t>90317880 - Lewis Mosciski
+ROLE : RTGO100 1701844270281</t>
+  </si>
+  <si>
+    <t>90833312 - Angelo Mueller
+ROLE : RTGO100 1701844270281</t>
+  </si>
+  <si>
+    <t>ROLE GROUP : RTGO Operator 2023-12-07T19:27:58.156908600</t>
+  </si>
+  <si>
+    <t>92970163 - Glenna Lynch
+ROLE : RTGO100 1701853905917</t>
   </si>
 </sst>
 </file>
@@ -463,32 +482,32 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
E10_2910_Workforce Employee Roster V2 Test for Build 159
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="21">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -507,17 +507,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Automation Test Report - Build v4.22.00.159
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="21">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -507,17 +507,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
New patch update on Build v4.22.00.159
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="29">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -132,6 +132,14 @@
   <si>
     <t>32695715 - Odell Carter
 ROLE : QCO 1705835784686</t>
+  </si>
+  <si>
+    <t>32426530 - Russel Bergstrom
+ROLE : QCO 1706020141934</t>
+  </si>
+  <si>
+    <t>32695715 - Odell Carter
+ROLE : QCO 1706021777804</t>
   </si>
 </sst>
 </file>
@@ -509,37 +517,37 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Execute All Module except ESS
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="31">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -144,6 +144,10 @@
   <si>
     <t>32426530 - Russel Bergstrom
 ROLE : QCO 1706083928031</t>
+  </si>
+  <si>
+    <t>13292186 - Lamont Champlin
+ROLE : QCO 1706187312887</t>
   </si>
 </sst>
 </file>
@@ -521,7 +525,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -531,32 +535,32 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Build Release-: V 4.24.0.160
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
+++ b/src/test/resources/TestData/Employee Roster V2_E10-2949.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="32">
   <si>
     <t>ROLE GROUP : RTGO Operator 2023-11-10T12:39:19.154601100</t>
   </si>
@@ -148,6 +148,10 @@
   <si>
     <t>13292186 - Lamont Champlin
 ROLE : QCO 1706187312887</t>
+  </si>
+  <si>
+    <t>68306525 - Danielle Gaylord
+ROLE : QCO 2023-11-24T09:25:13.428483500</t>
   </si>
 </sst>
 </file>
@@ -525,32 +529,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -560,7 +564,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">

</xml_diff>